<commit_message>
updated the third LGI homework finished the fourth LGI homework
</commit_message>
<xml_diff>
--- a/RWE/0_2016/exercises/1_Hauptbuch.xlsx
+++ b/RWE/0_2016/exercises/1_Hauptbuch.xlsx
@@ -9,19 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
-    <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
+    <sheet name="homework" sheetId="1" r:id="rId1"/>
+    <sheet name="20161105" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="31">
   <si>
     <t>Waren</t>
   </si>
@@ -99,12 +98,30 @@
   </si>
   <si>
     <t>SBK</t>
+  </si>
+  <si>
+    <t>Eröffnungsbilanz</t>
+  </si>
+  <si>
+    <t>SOLL</t>
+  </si>
+  <si>
+    <t>HABEN</t>
+  </si>
+  <si>
+    <t>Eröffnungsbilanzkonto</t>
+  </si>
+  <si>
+    <t>Lieferforderung</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;€&quot;\ #,##0.00"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -259,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -282,6 +299,9 @@
     <xf numFmtId="4" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -297,9 +317,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -640,8 +665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -679,14 +704,14 @@
       <c r="I3" s="18"/>
     </row>
     <row r="4" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
     </row>
     <row r="5" spans="1:9" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -766,14 +791,14 @@
       </c>
     </row>
     <row r="12" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
     </row>
     <row r="13" spans="1:9" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
@@ -858,22 +883,22 @@
       <c r="L17" s="19"/>
     </row>
     <row r="20" spans="1:13" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="H20" s="20" t="s">
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="H20" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="21"/>
-      <c r="M20" s="21"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
+      <c r="M20" s="24"/>
     </row>
     <row r="21" spans="1:13" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -935,32 +960,32 @@
       <c r="M23" s="5"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C24" s="25">
+      <c r="C24" s="20">
         <f>SUM(C21:C23)</f>
         <v>806000</v>
       </c>
-      <c r="F24" s="26">
+      <c r="F24" s="21">
         <f>SUM(F21:F23)</f>
         <v>806000</v>
       </c>
-      <c r="J24" s="26">
+      <c r="J24" s="21">
         <f>SUM(J21:J23)</f>
         <v>627000</v>
       </c>
-      <c r="M24" s="26">
+      <c r="M24" s="21">
         <f>SUM(M21:M23)</f>
         <v>627000</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H25" s="20" t="s">
+      <c r="H25" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="I25" s="21"/>
-      <c r="J25" s="21"/>
-      <c r="K25" s="21"/>
-      <c r="L25" s="21"/>
-      <c r="M25" s="21"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24"/>
+      <c r="L25" s="24"/>
+      <c r="M25" s="24"/>
     </row>
     <row r="26" spans="1:13" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="H26">
@@ -984,14 +1009,14 @@
       </c>
     </row>
     <row r="27" spans="1:13" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="20" t="s">
+      <c r="A27" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
       <c r="H27" t="s">
         <v>24</v>
       </c>
@@ -1044,21 +1069,21 @@
       <c r="F29" s="5">
         <v>82000</v>
       </c>
-      <c r="J29" s="26">
+      <c r="J29" s="21">
         <f>SUM(J26:J28)</f>
         <v>334000</v>
       </c>
-      <c r="M29" s="26">
+      <c r="M29" s="21">
         <f>SUM(M26:M28)</f>
         <v>334000</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C30" s="25">
+      <c r="C30" s="20">
         <f>SUM(C28:C29)</f>
         <v>124000</v>
       </c>
-      <c r="F30" s="26">
+      <c r="F30" s="21">
         <f>SUM(F28:F29)</f>
         <v>124000</v>
       </c>
@@ -1067,26 +1092,26 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C31" s="4"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
-      <c r="K31" s="24"/>
-      <c r="L31" s="24"/>
-      <c r="M31" s="24"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="27"/>
+      <c r="J31" s="27"/>
+      <c r="K31" s="27"/>
+      <c r="L31" s="27"/>
+      <c r="M31" s="27"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="J32" s="4"/>
       <c r="M32" s="5"/>
     </row>
     <row r="33" spans="1:13" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="20" t="s">
+      <c r="A33" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
       <c r="J33" s="4"/>
       <c r="M33" s="5"/>
     </row>
@@ -1142,22 +1167,22 @@
       <c r="M36" s="5"/>
     </row>
     <row r="37" spans="1:13" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="25">
+      <c r="C37" s="20">
         <f>SUM(C34:C36)</f>
         <v>31000</v>
       </c>
-      <c r="F37" s="26">
+      <c r="F37" s="21">
         <f>SUM(F34:F36)</f>
         <v>31000</v>
       </c>
-      <c r="H37" s="20" t="s">
+      <c r="H37" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="I37" s="21"/>
-      <c r="J37" s="21"/>
-      <c r="K37" s="21"/>
-      <c r="L37" s="21"/>
-      <c r="M37" s="21"/>
+      <c r="I37" s="24"/>
+      <c r="J37" s="24"/>
+      <c r="K37" s="24"/>
+      <c r="L37" s="24"/>
+      <c r="M37" s="24"/>
     </row>
     <row r="38" spans="1:13" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
@@ -1206,14 +1231,14 @@
       </c>
     </row>
     <row r="40" spans="1:13" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="20" t="s">
+      <c r="A40" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B40" s="21"/>
-      <c r="C40" s="21"/>
-      <c r="D40" s="21"/>
-      <c r="E40" s="21"/>
-      <c r="F40" s="21"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="24"/>
+      <c r="F40" s="24"/>
       <c r="H40" t="s">
         <v>24</v>
       </c>
@@ -1236,7 +1261,7 @@
       <c r="C41" s="2">
         <v>0</v>
       </c>
-      <c r="D41" s="27" t="s">
+      <c r="D41" s="22" t="s">
         <v>24</v>
       </c>
       <c r="E41" t="s">
@@ -1267,11 +1292,11 @@
       <c r="C42" s="3">
         <v>9000</v>
       </c>
-      <c r="J42" s="26">
+      <c r="J42" s="21">
         <f>SUM(J38:J41)</f>
         <v>948600</v>
       </c>
-      <c r="M42" s="26">
+      <c r="M42" s="21">
         <f>SUM(M38:M41)</f>
         <v>948600</v>
       </c>
@@ -1288,11 +1313,11 @@
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C44" s="25">
+      <c r="C44" s="20">
         <f>SUM(C41:C43)</f>
         <v>51000</v>
       </c>
-      <c r="F44" s="26">
+      <c r="F44" s="21">
         <f>SUM(F41:F43)</f>
         <v>51000</v>
       </c>
@@ -1322,28 +1347,520 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="29" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" style="29" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="29">
+        <v>710000</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="29">
+        <v>627000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="29">
+        <v>124000</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="29">
+        <v>238000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="29">
+        <v>31000</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="29">
+        <f>SUM(A3:A5)</f>
+        <v>865000</v>
+      </c>
+      <c r="D6" s="29">
+        <f>SUM(D3:D5)</f>
+        <v>865000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="29">
+        <v>627000</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="29">
+        <v>710000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="29">
+        <v>238000</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="29">
+        <v>124000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="29">
+        <v>31000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="29">
+        <f>SUM(A10:A11)</f>
+        <v>865000</v>
+      </c>
+      <c r="D13" s="29">
+        <f>SUM(D10:D12)</f>
+        <v>865000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="F15" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" s="31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="29">
+        <f>D10</f>
+        <v>710000</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" s="29">
+        <f>A10</f>
+        <v>627000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="29">
+        <v>96000</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="29">
+        <f>I17</f>
+        <v>627000</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C19" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="29">
+        <f>A20</f>
+        <v>806000</v>
+      </c>
+      <c r="F19" s="29">
+        <f>SUM(F17:F18)</f>
+        <v>627000</v>
+      </c>
+      <c r="I19" s="29">
+        <f>SUM(I17:I18)</f>
+        <v>627000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="29">
+        <f>SUM(A17:A19)</f>
+        <v>806000</v>
+      </c>
+      <c r="D20" s="29">
+        <f>SUM(D17:D19)</f>
+        <v>806000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="F23" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23" s="30"/>
+      <c r="H23" s="30"/>
+      <c r="I23" s="30"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="I24" s="31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="29">
+        <f>D11</f>
+        <v>124000</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="29">
+        <v>42000</v>
+      </c>
+      <c r="F25" s="29">
+        <v>12400</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I25" s="29">
+        <f>A11</f>
+        <v>238000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C26" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D26" s="29">
+        <f>A27-D25</f>
+        <v>82000</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I26" s="29">
+        <v>96000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="29">
+        <f>SUM(A25:A26)</f>
+        <v>124000</v>
+      </c>
+      <c r="D27" s="29">
+        <f>SUM(D25:D26)</f>
+        <v>124000</v>
+      </c>
+      <c r="F27" s="29">
+        <f>I28-F25</f>
+        <v>321600</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F28" s="29">
+        <f>SUM(F25:F27)</f>
+        <v>334000</v>
+      </c>
+      <c r="I28" s="29">
+        <f>SUM(I25:I27)</f>
+        <v>334000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="F31" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="G31" s="30"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="30"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="F32" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="H32" s="6"/>
+      <c r="I32" s="31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="29">
+        <f>D12</f>
+        <v>31000</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D33" s="29">
+        <v>9000</v>
+      </c>
+      <c r="F33" s="29">
+        <f>D35</f>
+        <v>9600</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I33" s="29">
+        <f>F27</f>
+        <v>321600</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C34" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="29">
+        <v>12400</v>
+      </c>
+      <c r="F34" s="29">
+        <f>D19</f>
+        <v>806000</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I34" s="29">
+        <f>F18</f>
+        <v>627000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C35" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D35" s="29">
+        <f>A36-(D34+D33)</f>
+        <v>9600</v>
+      </c>
+      <c r="F35" s="29">
+        <f>D26</f>
+        <v>82000</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="29">
+        <f>SUM(A33:A35)</f>
+        <v>31000</v>
+      </c>
+      <c r="D36" s="29">
+        <f>SUM(D33:D35)</f>
+        <v>31000</v>
+      </c>
+      <c r="F36" s="29">
+        <f>D44</f>
+        <v>51000</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F37" s="29">
+        <f>SUM(F33:F36)</f>
+        <v>948600</v>
+      </c>
+      <c r="I37" s="29">
+        <f>SUM(I33:I36)</f>
+        <v>948600</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B40" s="30"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="D41" s="31" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="29">
+        <v>9000</v>
+      </c>
+      <c r="B42" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="29">
+        <v>42000</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C44" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D44" s="29">
+        <f>A45</f>
+        <v>51000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="29">
+        <f>SUM(A42:A44)</f>
+        <v>51000</v>
+      </c>
+      <c r="D45" s="29">
+        <f>SUM(D42:D44)</f>
+        <v>51000</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="A40:D40"/>
+    <mergeCell ref="F31:I31"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A23:D23"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.4921259845" footer="0.4921259845"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.4921259845" footer="0.4921259845"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>